<commit_message>
Major structural changes and adding jupytext markdown versions
Decided to re-structure both notebooks to leave only the essentials needed to run searches (removed several sections from the python notebook specifically). Also, added better instructions on the R notebook, and markdown versions of both notebooks
</commit_message>
<xml_diff>
--- a/Keyword Searches/ABM & GW/Cleaning Files/NaN_Check_AU1_CO.xlsx
+++ b/Keyword Searches/ABM & GW/Cleaning Files/NaN_Check_AU1_CO.xlsx
@@ -1,108 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t>DI</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>AU1_CO</t>
-  </si>
-  <si>
-    <t>AU_CO</t>
-  </si>
-  <si>
-    <t>AU1_CO_NEW</t>
-  </si>
-  <si>
-    <t>10.4000/CYBERGEO.27475</t>
-  </si>
-  <si>
-    <t>10.1029/2018WR024180</t>
-  </si>
-  <si>
-    <t>10.1016/J.SCS.2019.101922</t>
-  </si>
-  <si>
-    <t>10.1016/J.GLOENVCHA.2012.10.002</t>
-  </si>
-  <si>
-    <t>POLLUTION TRANSFER IN GROUNDWATER USING A MULTIAGENTS SYSTEM TRANSFERT DUNE POLLUTION SOLUBLE DANS UN AQUIFRE PAR UNE APPROCHE MULTIAGENTS</t>
-  </si>
-  <si>
-    <t>EFFECT OF HYDROGEOLOGIC AND CLIMATIC VARIABILITY ON PERFORMANCE OF A GROUNDWATER MARKET</t>
-  </si>
-  <si>
-    <t>A COUPLED AGENTBASED RISKBASED OPTIMIZATION MODEL FOR INTEGRATED URBAN WATER MANAGEMENT</t>
-  </si>
-  <si>
-    <t>THE IMPACT OF URBANIZATION ON WATER VULNERABILITY A COUPLED HUMANENVIRONMENT SYSTEM APPROACH FOR CHENNAI INDIA</t>
-  </si>
-  <si>
-    <t>FLEURANT C</t>
-  </si>
-  <si>
-    <t>KHAN H;BROWN C</t>
-  </si>
-  <si>
-    <t>BAKHTIARI P;NIKOO M;IZADY A;TALEBBEYDOKHTI N</t>
-  </si>
-  <si>
-    <t>SRINIVASAN V;SETO K;EMERSON R;GORELICK S</t>
-  </si>
-  <si>
-    <t>FRANCE</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>OMAN</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,18 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -136,15 +57,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -433,102 +353,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>AU1_CO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AU_CO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>AU1_CO_NEW</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10.1002/2014WR016825</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>GLOBAL CHANGE AND THE GROUNDWATER MANAGEMENT CHALLENGE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>GORELICK S;ZHENG C</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.4000/CYBERGEO.27475</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>POLLUTION TRANSFER IN GROUNDWATER USING A MULTIAGENTS SYSTEM TRANSFERT DUNE POLLUTION SOLUBLE DANS UN AQUIFRE PAR UNE APPROCHE MULTIAGENTS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>FLEURANT C</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.12011/1000-6788(2017)12-3289-08</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>STUDY ON PARALLEL EMERGENCY MANAGEMENT METHOD FOR MINE WATER INRUSH</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>FENG Z;WANG T;GU Q;LU C;LI R;BAI Y</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CHINA</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10.1029/2018WR024180</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>EFFECT OF HYDROGEOLOGIC AND CLIMATIC VARIABILITY ON PERFORMANCE OF A GROUNDWATER MARKET</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>KHAN H;BROWN C</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10.11975/J.ISSN.1002-6819.2019.11.023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MONITORING CHLORPYRIFOS AND ABAMECTIN IN WATER BODIES OF PADDIES AND ASSESSMENT OF ECOLOGICAL RISK TO AQUATIC ANIMALS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CHEN C;LUO W;ZOU J;JIA Z;ZHANG Z;ZHU W</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CHINA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10.1016/J.SCS.2019.101922</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A COUPLED AGENTBASED RISKBASED OPTIMIZATION MODEL FOR INTEGRATED URBAN WATER MANAGEMENT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>BAKHTIARI P;NIKOO M;IZADY A;TALEBBEYDOKHTI N</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>OMAN</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>